<commit_message>
Consistent classification of data elements and data element contexts.
</commit_message>
<xml_diff>
--- a/import-files/sdtm-1-2.xlsx
+++ b/import-files/sdtm-1-2.xlsx
@@ -1295,381 +1295,6 @@
     <t>sdtm-1-2:Classifier.TimingVariable</t>
   </si>
   <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--TERM</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--MODIFY</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--DECOD</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--CAT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--SCAT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--PRESP</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--OCCUR</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--STAT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--REASND</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--BODSYS</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--LOC</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--SEV</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--SER</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--ACN</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--ACNOTH</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--REL</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--RELNST</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--PATT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--OUT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--SCAN</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--SCONG</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--SDISAB</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--SDTH</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--SHOSP</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--SLIFE</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--SOD</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--SMIE</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--CONTRT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--TOX</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Event.--TOXGR</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--TESTCD</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--TEST</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--MODIFY</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--CAT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--SCAT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--POS</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--BODSYS</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--ORRES</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--ORRESU</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--ORNRLO</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--ORNRHI</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--STRESC</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--STRESN</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--STRESU</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--STNRLO</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--STNRHI</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--STNRC</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--NRIND</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--RESCAT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--STAT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--REASND</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--XFN</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--NAM</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--LOINC</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--SPEC</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--SPCCND</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--LOC</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--METHOD</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--BLFL</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--FAST</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--DRVFL</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--EVAL</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--TOX</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--TOXGR</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--SEV</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--DTHREL</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Finding.--LLOQ</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.FindingAbout.--OBJ</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Identifier.STUDYID</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Identifier.DOMAIN</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Identifier.USUBJID</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Identifier.--SEQ</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Identifier.--GRPID</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Identifier.--REFID</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Identifier.--SPID</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--TRT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--MODIFY</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--DECOD</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--CAT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--SCAT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--PRESP</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--OCCUR</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--STAT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--REASND</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--INDC</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--CLAS</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--CLASCD</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--DOSE</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--DOSTXT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--DOSU</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--DOSFRM</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--DOSFRQ</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--DOSTOT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--DOSRGM</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--ROUTE</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--LOT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--LOC</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--TRTV</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--VAMT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--VAMTU</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Intervention.--ADJ</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.VISITNUM</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.VISIT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.VISITDY</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.TAETORD</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.EPOCH</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--DTC</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--STDTC</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--ENDTC</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--DY</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--STDY</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--ENDY</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--DUR</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--TPT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--TPTNUM</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--ELTM</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--TPTREF</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--RFTDTC</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--STRF</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--ENRF</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--EVLINT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--STRTPT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--STTPT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--ENRTPT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:sdtm-1-2:DE.Timing.--ENTPT</t>
-  </si>
-  <si>
     <t>sdtm-1-2:Classifier.RequiredVariable</t>
   </si>
   <si>
@@ -1761,6 +1386,381 @@
   </si>
   <si>
     <t>Variable Qualifiers are used to further modify or describe a specific variable within an observation and are only meaningful in the context of the variable they qualify. Examples include --ORRESU, --ORNRHI, and --ORNRLO, all of which are Variable Qualifiers of --ORRES; and --DOSU, which is a Variable Qualifier of --DOSE.</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--TERM</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--MODIFY</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--DECOD</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--CAT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--SCAT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--PRESP</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--OCCUR</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--STAT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--REASND</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--BODSYS</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--LOC</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--SEV</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--SER</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--ACN</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--ACNOTH</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--REL</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--RELNST</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--PATT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--OUT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--SCAN</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--SCONG</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--SDISAB</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--SDTH</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--SHOSP</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--SLIFE</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--SOD</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--SMIE</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--CONTRT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--TOX</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Event.--TOXGR</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--TESTCD</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--TEST</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--MODIFY</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--CAT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--SCAT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--POS</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--BODSYS</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--ORRES</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--ORRESU</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--ORNRLO</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--ORNRHI</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--STRESC</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--STRESN</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--STRESU</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--STNRLO</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--STNRHI</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--STNRC</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--NRIND</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--RESCAT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--STAT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--REASND</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--XFN</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--NAM</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--LOINC</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--SPEC</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--SPCCND</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--LOC</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--METHOD</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--BLFL</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--FAST</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--DRVFL</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--EVAL</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--TOX</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--TOXGR</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--SEV</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--DTHREL</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Finding.--LLOQ</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.FindingAbout.--OBJ</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Identifier.STUDYID</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Identifier.DOMAIN</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Identifier.USUBJID</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Identifier.--SEQ</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Identifier.--GRPID</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Identifier.--REFID</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Identifier.--SPID</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--TRT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--MODIFY</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--DECOD</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--CAT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--SCAT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--PRESP</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--OCCUR</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--STAT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--REASND</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--INDC</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--CLAS</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--CLASCD</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--DOSE</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--DOSTXT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--DOSU</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--DOSFRM</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--DOSFRQ</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--DOSTOT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--DOSRGM</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--ROUTE</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--LOT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--LOC</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--TRTV</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--VAMT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--VAMTU</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Intervention.--ADJ</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.VISITNUM</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.VISIT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.VISITDY</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.TAETORD</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.EPOCH</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--DTC</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--STDTC</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--ENDTC</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--DY</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--STDY</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--ENDY</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--DUR</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--TPT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--TPTNUM</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--ELTM</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--TPTREF</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--RFTDTC</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--STRF</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--ENRF</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--EVLINT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--STRTPT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--STTPT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--ENRTPT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--ENTPT</t>
   </si>
 </sst>
 </file>
@@ -2411,12 +2411,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -2428,6 +2422,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="538">
@@ -3301,7 +3301,7 @@
     <col min="1" max="1" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
@@ -3315,7 +3315,7 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>362</v>
       </c>
     </row>
@@ -3329,7 +3329,7 @@
       <c r="C2" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>365</v>
       </c>
     </row>
@@ -3359,19 +3359,19 @@
   <cols>
     <col min="1" max="1" width="35.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" style="6" customWidth="1"/>
     <col min="4" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>528</v>
+        <v>403</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>532</v>
+        <v>404</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="63.75">
@@ -3379,32 +3379,32 @@
         <v>381</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>531</v>
+        <v>405</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="76.5">
       <c r="A3" s="1" t="s">
-        <v>526</v>
+        <v>401</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>534</v>
+        <v>408</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="38.25">
       <c r="A4" s="1" t="s">
-        <v>525</v>
+        <v>400</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>536</v>
+        <v>410</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -3428,19 +3428,19 @@
   <cols>
     <col min="1" max="1" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" style="6" customWidth="1"/>
     <col min="4" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>537</v>
+        <v>412</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>532</v>
+        <v>404</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="25.5">
@@ -3448,10 +3448,10 @@
         <v>394</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>539</v>
+        <v>413</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="25.5">
@@ -3459,10 +3459,10 @@
         <v>398</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>541</v>
+        <v>415</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="51">
@@ -3470,10 +3470,10 @@
         <v>395</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>543</v>
+        <v>417</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="38.25">
@@ -3481,21 +3481,21 @@
         <v>397</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>545</v>
+        <v>419</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="25.5">
       <c r="A6" s="1" t="s">
-        <v>527</v>
+        <v>402</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>547</v>
+        <v>421</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="38.25">
@@ -3503,10 +3503,10 @@
         <v>393</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>549</v>
+        <v>423</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3514,10 +3514,10 @@
         <v>399</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>551</v>
+        <v>425</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3525,10 +3525,10 @@
         <v>392</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>553</v>
+        <v>427</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="51">
@@ -3536,10 +3536,10 @@
         <v>396</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>555</v>
+        <v>429</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -3563,7 +3563,7 @@
   <cols>
     <col min="1" max="1" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
@@ -3575,7 +3575,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -3589,7 +3589,7 @@
       <c r="B2" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="8">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -3603,7 +3603,7 @@
       <c r="B3" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -3617,7 +3617,7 @@
       <c r="B4" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -3631,7 +3631,7 @@
       <c r="B5" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -3645,7 +3645,7 @@
       <c r="B6" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -3659,7 +3659,7 @@
       <c r="B7" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="8">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -3690,13 +3690,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="81.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="81.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -3712,7 +3712,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -3724,7 +3724,7 @@
       <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -3744,13 +3744,13 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="25.5">
-      <c r="A2" s="3" t="s">
-        <v>400</v>
+      <c r="A2" s="1" t="s">
+        <v>431</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="8">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -3762,7 +3762,7 @@
       <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -3779,13 +3779,13 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="3" t="s">
-        <v>401</v>
+      <c r="A3" s="1" t="s">
+        <v>432</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -3797,7 +3797,7 @@
       <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -3817,13 +3817,13 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="38.25">
-      <c r="A4" s="3" t="s">
-        <v>402</v>
+      <c r="A4" s="1" t="s">
+        <v>433</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -3835,7 +3835,7 @@
       <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -3855,13 +3855,13 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="3" t="s">
-        <v>403</v>
+      <c r="A5" s="1" t="s">
+        <v>434</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -3873,7 +3873,7 @@
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -3890,13 +3890,13 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="3" t="s">
-        <v>404</v>
+      <c r="A6" s="1" t="s">
+        <v>435</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -3908,7 +3908,7 @@
       <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="6" t="s">
         <v>25</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -3925,13 +3925,13 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="25.5">
-      <c r="A7" s="3" t="s">
-        <v>405</v>
+      <c r="A7" s="1" t="s">
+        <v>436</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="8">
         <v>6</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -3943,7 +3943,7 @@
       <c r="F7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="6" t="s">
         <v>27</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -3960,13 +3960,13 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="25.5">
-      <c r="A8" s="3" t="s">
-        <v>406</v>
+      <c r="A8" s="1" t="s">
+        <v>437</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="8">
         <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -3978,7 +3978,7 @@
       <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="6" t="s">
         <v>29</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -3995,13 +3995,13 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="25.5">
-      <c r="A9" s="3" t="s">
-        <v>407</v>
+      <c r="A9" s="1" t="s">
+        <v>438</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="8">
         <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -4013,7 +4013,7 @@
       <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="6" t="s">
         <v>31</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -4030,13 +4030,13 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="3" t="s">
-        <v>408</v>
+      <c r="A10" s="1" t="s">
+        <v>439</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="8">
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -4048,7 +4048,7 @@
       <c r="F10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -4065,13 +4065,13 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="25.5">
-      <c r="A11" s="3" t="s">
-        <v>409</v>
+      <c r="A11" s="1" t="s">
+        <v>440</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="8">
         <v>10</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -4083,7 +4083,7 @@
       <c r="F11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="6" t="s">
         <v>35</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -4100,13 +4100,13 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="3" t="s">
-        <v>410</v>
+      <c r="A12" s="1" t="s">
+        <v>441</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="8">
         <v>11</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -4118,7 +4118,7 @@
       <c r="F12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="6" t="s">
         <v>37</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -4135,13 +4135,13 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="3" t="s">
-        <v>411</v>
+      <c r="A13" s="1" t="s">
+        <v>442</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="8">
         <v>12</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -4153,7 +4153,7 @@
       <c r="F13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="6" t="s">
         <v>39</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -4170,13 +4170,13 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="3" t="s">
-        <v>412</v>
+      <c r="A14" s="1" t="s">
+        <v>443</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="8">
         <v>13</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -4188,7 +4188,7 @@
       <c r="F14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="6" t="s">
         <v>41</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -4205,13 +4205,13 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="25.5">
-      <c r="A15" s="3" t="s">
-        <v>413</v>
+      <c r="A15" s="1" t="s">
+        <v>444</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="8">
         <v>14</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -4223,7 +4223,7 @@
       <c r="F15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="6" t="s">
         <v>43</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -4240,13 +4240,13 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="25.5">
-      <c r="A16" s="3" t="s">
-        <v>414</v>
+      <c r="A16" s="1" t="s">
+        <v>445</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="8">
         <v>15</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -4258,7 +4258,7 @@
       <c r="F16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="6" t="s">
         <v>45</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -4275,13 +4275,13 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="38.25">
-      <c r="A17" s="3" t="s">
-        <v>415</v>
+      <c r="A17" s="1" t="s">
+        <v>446</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="8">
         <v>16</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -4293,7 +4293,7 @@
       <c r="F17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="6" t="s">
         <v>47</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -4310,13 +4310,13 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="25.5">
-      <c r="A18" s="3" t="s">
-        <v>416</v>
+      <c r="A18" s="1" t="s">
+        <v>447</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="8">
         <v>17</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -4328,7 +4328,7 @@
       <c r="F18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="6" t="s">
         <v>49</v>
       </c>
       <c r="H18" s="1" t="s">
@@ -4345,13 +4345,13 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="25.5">
-      <c r="A19" s="3" t="s">
-        <v>417</v>
+      <c r="A19" s="1" t="s">
+        <v>448</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="8">
         <v>18</v>
       </c>
       <c r="D19" s="4" t="s">
@@ -4363,7 +4363,7 @@
       <c r="F19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="6" t="s">
         <v>51</v>
       </c>
       <c r="H19" s="1" t="s">
@@ -4380,13 +4380,13 @@
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="3" t="s">
-        <v>418</v>
+      <c r="A20" s="1" t="s">
+        <v>449</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="8">
         <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
@@ -4398,7 +4398,7 @@
       <c r="F20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="6" t="s">
         <v>53</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -4415,13 +4415,13 @@
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="3" t="s">
-        <v>419</v>
+      <c r="A21" s="1" t="s">
+        <v>450</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="8">
         <v>20</v>
       </c>
       <c r="D21" s="4" t="s">
@@ -4433,7 +4433,7 @@
       <c r="F21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="6" t="s">
         <v>55</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -4450,13 +4450,13 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="25.5">
-      <c r="A22" s="3" t="s">
-        <v>420</v>
+      <c r="A22" s="1" t="s">
+        <v>451</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="8">
         <v>21</v>
       </c>
       <c r="D22" s="4" t="s">
@@ -4468,7 +4468,7 @@
       <c r="F22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="6" t="s">
         <v>57</v>
       </c>
       <c r="H22" s="1" t="s">
@@ -4485,13 +4485,13 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="25.5">
-      <c r="A23" s="3" t="s">
-        <v>421</v>
+      <c r="A23" s="1" t="s">
+        <v>452</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="8">
         <v>22</v>
       </c>
       <c r="D23" s="4" t="s">
@@ -4503,7 +4503,7 @@
       <c r="F23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="6" t="s">
         <v>59</v>
       </c>
       <c r="H23" s="1" t="s">
@@ -4520,13 +4520,13 @@
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="3" t="s">
-        <v>422</v>
+      <c r="A24" s="1" t="s">
+        <v>453</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="8">
         <v>23</v>
       </c>
       <c r="D24" s="4" t="s">
@@ -4538,7 +4538,7 @@
       <c r="F24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="6" t="s">
         <v>61</v>
       </c>
       <c r="H24" s="1" t="s">
@@ -4555,13 +4555,13 @@
       </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="3" t="s">
-        <v>423</v>
+      <c r="A25" s="1" t="s">
+        <v>454</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="8">
         <v>24</v>
       </c>
       <c r="D25" s="4" t="s">
@@ -4573,7 +4573,7 @@
       <c r="F25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="6" t="s">
         <v>63</v>
       </c>
       <c r="H25" s="1" t="s">
@@ -4590,13 +4590,13 @@
       </c>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="3" t="s">
-        <v>424</v>
+      <c r="A26" s="1" t="s">
+        <v>455</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="8">
         <v>25</v>
       </c>
       <c r="D26" s="4" t="s">
@@ -4608,7 +4608,7 @@
       <c r="F26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="6" t="s">
         <v>65</v>
       </c>
       <c r="H26" s="1" t="s">
@@ -4625,13 +4625,13 @@
       </c>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="3" t="s">
-        <v>425</v>
+      <c r="A27" s="1" t="s">
+        <v>456</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="8">
         <v>26</v>
       </c>
       <c r="D27" s="4" t="s">
@@ -4643,7 +4643,7 @@
       <c r="F27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="6" t="s">
         <v>67</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -4660,13 +4660,13 @@
       </c>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="3" t="s">
-        <v>426</v>
+      <c r="A28" s="1" t="s">
+        <v>457</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="8">
         <v>27</v>
       </c>
       <c r="D28" s="4" t="s">
@@ -4678,7 +4678,7 @@
       <c r="F28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="6" t="s">
         <v>69</v>
       </c>
       <c r="H28" s="1" t="s">
@@ -4695,13 +4695,13 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="25.5">
-      <c r="A29" s="3" t="s">
-        <v>427</v>
+      <c r="A29" s="1" t="s">
+        <v>458</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="8">
         <v>28</v>
       </c>
       <c r="D29" s="4" t="s">
@@ -4713,7 +4713,7 @@
       <c r="F29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H29" s="1" t="s">
@@ -4730,13 +4730,13 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="38.25">
-      <c r="A30" s="3" t="s">
-        <v>428</v>
+      <c r="A30" s="1" t="s">
+        <v>459</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="8">
         <v>29</v>
       </c>
       <c r="D30" s="4" t="s">
@@ -4748,7 +4748,7 @@
       <c r="F30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="G30" s="6" t="s">
         <v>73</v>
       </c>
       <c r="H30" s="1" t="s">
@@ -4768,13 +4768,13 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="38.25">
-      <c r="A31" s="3" t="s">
-        <v>429</v>
+      <c r="A31" s="1" t="s">
+        <v>460</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="8">
         <v>30</v>
       </c>
       <c r="D31" s="4" t="s">
@@ -4786,7 +4786,7 @@
       <c r="F31" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G31" s="6" t="s">
         <v>75</v>
       </c>
       <c r="H31" s="1" t="s">
@@ -4803,13 +4803,13 @@
       </c>
     </row>
     <row r="32" spans="1:12" ht="38.25">
-      <c r="A32" s="3" t="s">
-        <v>430</v>
+      <c r="A32" s="1" t="s">
+        <v>461</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="8">
         <v>1</v>
       </c>
       <c r="D32" s="4" t="s">
@@ -4821,7 +4821,7 @@
       <c r="F32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G32" s="6" t="s">
         <v>77</v>
       </c>
       <c r="H32" s="1" t="s">
@@ -4838,13 +4838,13 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="25.5">
-      <c r="A33" s="3" t="s">
-        <v>431</v>
+      <c r="A33" s="1" t="s">
+        <v>462</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="8">
         <v>2</v>
       </c>
       <c r="D33" s="4" t="s">
@@ -4856,7 +4856,7 @@
       <c r="F33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G33" s="6" t="s">
         <v>79</v>
       </c>
       <c r="H33" s="1" t="s">
@@ -4876,13 +4876,13 @@
       </c>
     </row>
     <row r="34" spans="1:12" ht="25.5">
-      <c r="A34" s="5" t="s">
-        <v>432</v>
+      <c r="A34" s="9" t="s">
+        <v>463</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="8">
         <v>3</v>
       </c>
       <c r="D34" s="4" t="s">
@@ -4894,7 +4894,7 @@
       <c r="F34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G34" s="6" t="s">
         <v>81</v>
       </c>
       <c r="H34" s="1" t="s">
@@ -4914,13 +4914,13 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="25.5">
-      <c r="A35" s="5" t="s">
-        <v>433</v>
+      <c r="A35" s="9" t="s">
+        <v>464</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="8">
         <v>4</v>
       </c>
       <c r="D35" s="4" t="s">
@@ -4932,7 +4932,7 @@
       <c r="F35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G35" s="6" t="s">
         <v>82</v>
       </c>
       <c r="H35" s="1" t="s">
@@ -4949,13 +4949,13 @@
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="5" t="s">
-        <v>434</v>
+      <c r="A36" s="9" t="s">
+        <v>465</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="8">
         <v>5</v>
       </c>
       <c r="D36" s="4" t="s">
@@ -4967,7 +4967,7 @@
       <c r="F36" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G36" s="6" t="s">
         <v>83</v>
       </c>
       <c r="H36" s="1" t="s">
@@ -4984,13 +4984,13 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="25.5">
-      <c r="A37" s="5" t="s">
-        <v>435</v>
+      <c r="A37" s="9" t="s">
+        <v>466</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="8">
         <v>6</v>
       </c>
       <c r="D37" s="4" t="s">
@@ -5002,7 +5002,7 @@
       <c r="F37" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G37" s="8" t="s">
+      <c r="G37" s="6" t="s">
         <v>85</v>
       </c>
       <c r="H37" s="1" t="s">
@@ -5019,13 +5019,13 @@
       </c>
     </row>
     <row r="38" spans="1:12" ht="25.5">
-      <c r="A38" s="5" t="s">
-        <v>436</v>
+      <c r="A38" s="9" t="s">
+        <v>467</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="8">
         <v>7</v>
       </c>
       <c r="D38" s="4" t="s">
@@ -5037,7 +5037,7 @@
       <c r="F38" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="8" t="s">
+      <c r="G38" s="6" t="s">
         <v>86</v>
       </c>
       <c r="H38" s="1" t="s">
@@ -5054,13 +5054,13 @@
       </c>
     </row>
     <row r="39" spans="1:12" ht="25.5">
-      <c r="A39" s="5" t="s">
-        <v>437</v>
+      <c r="A39" s="9" t="s">
+        <v>468</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="8">
         <v>8</v>
       </c>
       <c r="D39" s="4" t="s">
@@ -5072,7 +5072,7 @@
       <c r="F39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="8" t="s">
+      <c r="G39" s="6" t="s">
         <v>88</v>
       </c>
       <c r="H39" s="1" t="s">
@@ -5089,13 +5089,13 @@
       </c>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="5" t="s">
-        <v>438</v>
+      <c r="A40" s="9" t="s">
+        <v>469</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="8">
         <v>9</v>
       </c>
       <c r="D40" s="4" t="s">
@@ -5107,7 +5107,7 @@
       <c r="F40" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G40" s="8" t="s">
+      <c r="G40" s="6" t="s">
         <v>90</v>
       </c>
       <c r="H40" s="1" t="s">
@@ -5127,13 +5127,13 @@
       </c>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="5" t="s">
-        <v>439</v>
+      <c r="A41" s="9" t="s">
+        <v>470</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="8">
         <v>10</v>
       </c>
       <c r="D41" s="4" t="s">
@@ -5145,7 +5145,7 @@
       <c r="F41" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G41" s="8" t="s">
+      <c r="G41" s="6" t="s">
         <v>92</v>
       </c>
       <c r="H41" s="1" t="s">
@@ -5165,13 +5165,13 @@
       </c>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="5" t="s">
-        <v>440</v>
+      <c r="A42" s="9" t="s">
+        <v>471</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="8">
         <v>11</v>
       </c>
       <c r="D42" s="4" t="s">
@@ -5183,7 +5183,7 @@
       <c r="F42" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G42" s="8" t="s">
+      <c r="G42" s="6" t="s">
         <v>94</v>
       </c>
       <c r="H42" s="1" t="s">
@@ -5203,13 +5203,13 @@
       </c>
     </row>
     <row r="43" spans="1:12" ht="76.5">
-      <c r="A43" s="5" t="s">
-        <v>441</v>
+      <c r="A43" s="9" t="s">
+        <v>472</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="8">
         <v>12</v>
       </c>
       <c r="D43" s="4" t="s">
@@ -5221,7 +5221,7 @@
       <c r="F43" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G43" s="8" t="s">
+      <c r="G43" s="6" t="s">
         <v>96</v>
       </c>
       <c r="H43" s="1" t="s">
@@ -5238,13 +5238,13 @@
       </c>
     </row>
     <row r="44" spans="1:12" ht="25.5">
-      <c r="A44" s="5" t="s">
-        <v>442</v>
+      <c r="A44" s="9" t="s">
+        <v>473</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="8">
         <v>13</v>
       </c>
       <c r="D44" s="4" t="s">
@@ -5256,7 +5256,7 @@
       <c r="F44" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G44" s="8" t="s">
+      <c r="G44" s="6" t="s">
         <v>99</v>
       </c>
       <c r="H44" s="1" t="s">
@@ -5273,13 +5273,13 @@
       </c>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="5" t="s">
-        <v>443</v>
+      <c r="A45" s="9" t="s">
+        <v>474</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="8">
         <v>14</v>
       </c>
       <c r="D45" s="4" t="s">
@@ -5291,7 +5291,7 @@
       <c r="F45" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G45" s="8" t="s">
+      <c r="G45" s="6" t="s">
         <v>101</v>
       </c>
       <c r="H45" s="1" t="s">
@@ -5311,8 +5311,8 @@
       </c>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="6" t="s">
-        <v>443</v>
+      <c r="A46" s="10" t="s">
+        <v>474</v>
       </c>
       <c r="I46" s="3" t="s">
         <v>378</v>
@@ -5322,13 +5322,13 @@
       </c>
     </row>
     <row r="47" spans="1:12" ht="25.5">
-      <c r="A47" s="5" t="s">
-        <v>444</v>
+      <c r="A47" s="9" t="s">
+        <v>475</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="8">
         <v>15</v>
       </c>
       <c r="D47" s="4" t="s">
@@ -5340,7 +5340,7 @@
       <c r="F47" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G47" s="8" t="s">
+      <c r="G47" s="6" t="s">
         <v>103</v>
       </c>
       <c r="H47" s="1" t="s">
@@ -5360,8 +5360,8 @@
       </c>
     </row>
     <row r="48" spans="1:12">
-      <c r="A48" s="6" t="s">
-        <v>444</v>
+      <c r="A48" s="10" t="s">
+        <v>475</v>
       </c>
       <c r="I48" s="3" t="s">
         <v>378</v>
@@ -5371,13 +5371,13 @@
       </c>
     </row>
     <row r="49" spans="1:12" ht="25.5">
-      <c r="A49" s="5" t="s">
-        <v>445</v>
+      <c r="A49" s="9" t="s">
+        <v>476</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C49" s="10">
+      <c r="C49" s="8">
         <v>16</v>
       </c>
       <c r="D49" s="4" t="s">
@@ -5389,7 +5389,7 @@
       <c r="F49" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G49" s="8" t="s">
+      <c r="G49" s="6" t="s">
         <v>105</v>
       </c>
       <c r="H49" s="1" t="s">
@@ -5409,8 +5409,8 @@
       </c>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="6" t="s">
-        <v>445</v>
+      <c r="A50" s="10" t="s">
+        <v>476</v>
       </c>
       <c r="I50" s="3" t="s">
         <v>378</v>
@@ -5420,13 +5420,13 @@
       </c>
     </row>
     <row r="51" spans="1:12" ht="25.5">
-      <c r="A51" s="5" t="s">
-        <v>446</v>
+      <c r="A51" s="9" t="s">
+        <v>477</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C51" s="10">
+      <c r="C51" s="8">
         <v>17</v>
       </c>
       <c r="D51" s="4" t="s">
@@ -5438,7 +5438,7 @@
       <c r="F51" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G51" s="8" t="s">
+      <c r="G51" s="6" t="s">
         <v>107</v>
       </c>
       <c r="H51" s="1" t="s">
@@ -5458,13 +5458,13 @@
       </c>
     </row>
     <row r="52" spans="1:12" ht="38.25">
-      <c r="A52" s="5" t="s">
-        <v>447</v>
+      <c r="A52" s="9" t="s">
+        <v>478</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C52" s="10">
+      <c r="C52" s="8">
         <v>18</v>
       </c>
       <c r="D52" s="4" t="s">
@@ -5476,7 +5476,7 @@
       <c r="F52" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G52" s="8" t="s">
+      <c r="G52" s="6" t="s">
         <v>109</v>
       </c>
       <c r="H52" s="1" t="s">
@@ -5496,13 +5496,13 @@
       </c>
     </row>
     <row r="53" spans="1:12" ht="25.5">
-      <c r="A53" s="5" t="s">
-        <v>448</v>
+      <c r="A53" s="9" t="s">
+        <v>479</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C53" s="10">
+      <c r="C53" s="8">
         <v>19</v>
       </c>
       <c r="D53" s="4" t="s">
@@ -5514,7 +5514,7 @@
       <c r="F53" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G53" s="8" t="s">
+      <c r="G53" s="6" t="s">
         <v>111</v>
       </c>
       <c r="H53" s="1" t="s">
@@ -5534,13 +5534,13 @@
       </c>
     </row>
     <row r="54" spans="1:12" ht="25.5">
-      <c r="A54" s="5" t="s">
-        <v>449</v>
+      <c r="A54" s="9" t="s">
+        <v>480</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C54" s="10">
+      <c r="C54" s="8">
         <v>20</v>
       </c>
       <c r="D54" s="4" t="s">
@@ -5552,7 +5552,7 @@
       <c r="F54" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G54" s="8" t="s">
+      <c r="G54" s="6" t="s">
         <v>112</v>
       </c>
       <c r="H54" s="1" t="s">
@@ -5569,13 +5569,13 @@
       </c>
     </row>
     <row r="55" spans="1:12">
-      <c r="A55" s="5" t="s">
-        <v>450</v>
+      <c r="A55" s="9" t="s">
+        <v>481</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C55" s="10">
+      <c r="C55" s="8">
         <v>21</v>
       </c>
       <c r="D55" s="4" t="s">
@@ -5587,7 +5587,7 @@
       <c r="F55" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G55" s="8" t="s">
+      <c r="G55" s="6" t="s">
         <v>113</v>
       </c>
       <c r="H55" s="1" t="s">
@@ -5604,13 +5604,13 @@
       </c>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="5" t="s">
-        <v>451</v>
+      <c r="A56" s="9" t="s">
+        <v>482</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C56" s="10">
+      <c r="C56" s="8">
         <v>22</v>
       </c>
       <c r="D56" s="4" t="s">
@@ -5622,7 +5622,7 @@
       <c r="F56" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G56" s="8" t="s">
+      <c r="G56" s="6" t="s">
         <v>115</v>
       </c>
       <c r="H56" s="1" t="s">
@@ -5639,13 +5639,13 @@
       </c>
     </row>
     <row r="57" spans="1:12">
-      <c r="A57" s="5" t="s">
-        <v>452</v>
+      <c r="A57" s="9" t="s">
+        <v>483</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C57" s="10">
+      <c r="C57" s="8">
         <v>23</v>
       </c>
       <c r="D57" s="4" t="s">
@@ -5657,7 +5657,7 @@
       <c r="F57" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G57" s="8" t="s">
+      <c r="G57" s="6" t="s">
         <v>117</v>
       </c>
       <c r="H57" s="1" t="s">
@@ -5674,13 +5674,13 @@
       </c>
     </row>
     <row r="58" spans="1:12" ht="25.5">
-      <c r="A58" s="5" t="s">
-        <v>453</v>
+      <c r="A58" s="9" t="s">
+        <v>484</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C58" s="10">
+      <c r="C58" s="8">
         <v>24</v>
       </c>
       <c r="D58" s="4" t="s">
@@ -5692,7 +5692,7 @@
       <c r="F58" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G58" s="8" t="s">
+      <c r="G58" s="6" t="s">
         <v>119</v>
       </c>
       <c r="H58" s="1" t="s">
@@ -5712,13 +5712,13 @@
       </c>
     </row>
     <row r="59" spans="1:12" ht="25.5">
-      <c r="A59" s="5" t="s">
-        <v>454</v>
+      <c r="A59" s="9" t="s">
+        <v>485</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C59" s="10">
+      <c r="C59" s="8">
         <v>25</v>
       </c>
       <c r="D59" s="4" t="s">
@@ -5730,7 +5730,7 @@
       <c r="F59" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G59" s="8" t="s">
+      <c r="G59" s="6" t="s">
         <v>121</v>
       </c>
       <c r="H59" s="1" t="s">
@@ -5747,13 +5747,13 @@
       </c>
     </row>
     <row r="60" spans="1:12">
-      <c r="A60" s="5" t="s">
-        <v>455</v>
+      <c r="A60" s="9" t="s">
+        <v>486</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C60" s="10">
+      <c r="C60" s="8">
         <v>26</v>
       </c>
       <c r="D60" s="4" t="s">
@@ -5765,7 +5765,7 @@
       <c r="F60" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G60" s="8" t="s">
+      <c r="G60" s="6" t="s">
         <v>123</v>
       </c>
       <c r="H60" s="1" t="s">
@@ -5782,13 +5782,13 @@
       </c>
     </row>
     <row r="61" spans="1:12" ht="25.5">
-      <c r="A61" s="5" t="s">
-        <v>456</v>
+      <c r="A61" s="9" t="s">
+        <v>487</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C61" s="10">
+      <c r="C61" s="8">
         <v>27</v>
       </c>
       <c r="D61" s="4" t="s">
@@ -5800,7 +5800,7 @@
       <c r="F61" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G61" s="8" t="s">
+      <c r="G61" s="6" t="s">
         <v>125</v>
       </c>
       <c r="H61" s="1" t="s">
@@ -5817,13 +5817,13 @@
       </c>
     </row>
     <row r="62" spans="1:12" ht="25.5">
-      <c r="A62" s="5" t="s">
-        <v>457</v>
+      <c r="A62" s="9" t="s">
+        <v>488</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C62" s="10">
+      <c r="C62" s="8">
         <v>28</v>
       </c>
       <c r="D62" s="4" t="s">
@@ -5835,7 +5835,7 @@
       <c r="F62" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G62" s="8" t="s">
+      <c r="G62" s="6" t="s">
         <v>127</v>
       </c>
       <c r="H62" s="1" t="s">
@@ -5852,13 +5852,13 @@
       </c>
     </row>
     <row r="63" spans="1:12">
-      <c r="A63" s="5" t="s">
-        <v>458</v>
+      <c r="A63" s="9" t="s">
+        <v>489</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C63" s="10">
+      <c r="C63" s="8">
         <v>29</v>
       </c>
       <c r="D63" s="4" t="s">
@@ -5870,7 +5870,7 @@
       <c r="F63" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G63" s="8" t="s">
+      <c r="G63" s="6" t="s">
         <v>129</v>
       </c>
       <c r="H63" s="1" t="s">
@@ -5887,13 +5887,13 @@
       </c>
     </row>
     <row r="64" spans="1:12">
-      <c r="A64" s="5" t="s">
-        <v>459</v>
+      <c r="A64" s="9" t="s">
+        <v>490</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C64" s="10">
+      <c r="C64" s="8">
         <v>30</v>
       </c>
       <c r="D64" s="4" t="s">
@@ -5905,7 +5905,7 @@
       <c r="F64" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G64" s="8" t="s">
+      <c r="G64" s="6" t="s">
         <v>131</v>
       </c>
       <c r="H64" s="1" t="s">
@@ -5922,13 +5922,13 @@
       </c>
     </row>
     <row r="65" spans="1:12" ht="25.5">
-      <c r="A65" s="5" t="s">
-        <v>460</v>
+      <c r="A65" s="9" t="s">
+        <v>491</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C65" s="10">
+      <c r="C65" s="8">
         <v>31</v>
       </c>
       <c r="D65" s="4" t="s">
@@ -5940,7 +5940,7 @@
       <c r="F65" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G65" s="8" t="s">
+      <c r="G65" s="6" t="s">
         <v>133</v>
       </c>
       <c r="H65" s="1" t="s">
@@ -5957,13 +5957,13 @@
       </c>
     </row>
     <row r="66" spans="1:12" ht="38.25">
-      <c r="A66" s="5" t="s">
-        <v>461</v>
+      <c r="A66" s="9" t="s">
+        <v>492</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C66" s="10">
+      <c r="C66" s="8">
         <v>32</v>
       </c>
       <c r="D66" s="4" t="s">
@@ -5975,7 +5975,7 @@
       <c r="F66" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G66" s="8" t="s">
+      <c r="G66" s="6" t="s">
         <v>135</v>
       </c>
       <c r="H66" s="1" t="s">
@@ -5992,13 +5992,13 @@
       </c>
     </row>
     <row r="67" spans="1:12" ht="38.25">
-      <c r="A67" s="5" t="s">
-        <v>462</v>
+      <c r="A67" s="9" t="s">
+        <v>493</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C67" s="10">
+      <c r="C67" s="8">
         <v>33</v>
       </c>
       <c r="D67" s="4" t="s">
@@ -6010,7 +6010,7 @@
       <c r="F67" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G67" s="8" t="s">
+      <c r="G67" s="6" t="s">
         <v>73</v>
       </c>
       <c r="H67" s="1" t="s">
@@ -6030,13 +6030,13 @@
       </c>
     </row>
     <row r="68" spans="1:12" ht="38.25">
-      <c r="A68" s="5" t="s">
-        <v>463</v>
+      <c r="A68" s="9" t="s">
+        <v>494</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C68" s="10">
+      <c r="C68" s="8">
         <v>34</v>
       </c>
       <c r="D68" s="4" t="s">
@@ -6048,7 +6048,7 @@
       <c r="F68" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G68" s="8" t="s">
+      <c r="G68" s="6" t="s">
         <v>136</v>
       </c>
       <c r="H68" s="1" t="s">
@@ -6068,13 +6068,13 @@
       </c>
     </row>
     <row r="69" spans="1:12" ht="25.5">
-      <c r="A69" s="5" t="s">
-        <v>464</v>
+      <c r="A69" s="9" t="s">
+        <v>495</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C69" s="10">
+      <c r="C69" s="8">
         <v>35</v>
       </c>
       <c r="D69" s="4" t="s">
@@ -6086,7 +6086,7 @@
       <c r="F69" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G69" s="8" t="s">
+      <c r="G69" s="6" t="s">
         <v>138</v>
       </c>
       <c r="H69" s="1" t="s">
@@ -6103,13 +6103,13 @@
       </c>
     </row>
     <row r="70" spans="1:12">
-      <c r="A70" s="5" t="s">
-        <v>465</v>
+      <c r="A70" s="9" t="s">
+        <v>496</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C70" s="10">
+      <c r="C70" s="8">
         <v>36</v>
       </c>
       <c r="D70" s="4" t="s">
@@ -6121,7 +6121,7 @@
       <c r="F70" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G70" s="8" t="s">
+      <c r="G70" s="6" t="s">
         <v>140</v>
       </c>
       <c r="H70" s="1" t="s">
@@ -6138,13 +6138,13 @@
       </c>
     </row>
     <row r="71" spans="1:12">
-      <c r="A71" s="5" t="s">
-        <v>466</v>
+      <c r="A71" s="9" t="s">
+        <v>497</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C71" s="10">
+      <c r="C71" s="8">
         <v>37</v>
       </c>
       <c r="D71" s="4" t="s">
@@ -6156,7 +6156,7 @@
       <c r="F71" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G71" s="8" t="s">
+      <c r="G71" s="6" t="s">
         <v>142</v>
       </c>
       <c r="H71" s="1" t="s">
@@ -6176,13 +6176,13 @@
       </c>
     </row>
     <row r="72" spans="1:12" ht="51">
-      <c r="A72" s="3" t="s">
-        <v>467</v>
+      <c r="A72" s="1" t="s">
+        <v>498</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="C72" s="10">
+      <c r="C72" s="8">
         <v>1</v>
       </c>
       <c r="D72" s="4" t="s">
@@ -6194,7 +6194,7 @@
       <c r="F72" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G72" s="8" t="s">
+      <c r="G72" s="6" t="s">
         <v>144</v>
       </c>
       <c r="H72" s="1" t="s">
@@ -6211,13 +6211,13 @@
       </c>
     </row>
     <row r="73" spans="1:12">
-      <c r="A73" s="3" t="s">
-        <v>468</v>
+      <c r="A73" s="1" t="s">
+        <v>499</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C73" s="10">
+      <c r="C73" s="8">
         <v>1</v>
       </c>
       <c r="D73" s="3" t="s">
@@ -6229,7 +6229,7 @@
       <c r="F73" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G73" s="8" t="s">
+      <c r="G73" s="6" t="s">
         <v>147</v>
       </c>
       <c r="H73" s="1" t="s">
@@ -6246,13 +6246,13 @@
       </c>
     </row>
     <row r="74" spans="1:12" ht="38.25">
-      <c r="A74" s="3" t="s">
-        <v>469</v>
+      <c r="A74" s="1" t="s">
+        <v>500</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C74" s="10">
+      <c r="C74" s="8">
         <v>2</v>
       </c>
       <c r="D74" s="3" t="s">
@@ -6264,7 +6264,7 @@
       <c r="F74" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G74" s="8" t="s">
+      <c r="G74" s="6" t="s">
         <v>150</v>
       </c>
       <c r="H74" s="1" t="s">
@@ -6281,13 +6281,13 @@
       </c>
     </row>
     <row r="75" spans="1:12" ht="25.5">
-      <c r="A75" s="3" t="s">
-        <v>470</v>
+      <c r="A75" s="1" t="s">
+        <v>501</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C75" s="10">
+      <c r="C75" s="8">
         <v>3</v>
       </c>
       <c r="D75" s="3" t="s">
@@ -6299,7 +6299,7 @@
       <c r="F75" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G75" s="8" t="s">
+      <c r="G75" s="6" t="s">
         <v>153</v>
       </c>
       <c r="H75" s="1" t="s">
@@ -6316,13 +6316,13 @@
       </c>
     </row>
     <row r="76" spans="1:12" ht="51">
-      <c r="A76" s="3" t="s">
-        <v>471</v>
+      <c r="A76" s="1" t="s">
+        <v>502</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C76" s="10">
+      <c r="C76" s="8">
         <v>4</v>
       </c>
       <c r="D76" s="4" t="s">
@@ -6334,7 +6334,7 @@
       <c r="F76" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G76" s="8" t="s">
+      <c r="G76" s="6" t="s">
         <v>155</v>
       </c>
       <c r="H76" s="1" t="s">
@@ -6351,13 +6351,13 @@
       </c>
     </row>
     <row r="77" spans="1:12" ht="25.5">
-      <c r="A77" s="3" t="s">
-        <v>472</v>
+      <c r="A77" s="1" t="s">
+        <v>503</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C77" s="10">
+      <c r="C77" s="8">
         <v>5</v>
       </c>
       <c r="D77" s="4" t="s">
@@ -6369,7 +6369,7 @@
       <c r="F77" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G77" s="8" t="s">
+      <c r="G77" s="6" t="s">
         <v>157</v>
       </c>
       <c r="H77" s="1" t="s">
@@ -6386,13 +6386,13 @@
       </c>
     </row>
     <row r="78" spans="1:12" ht="25.5">
-      <c r="A78" s="3" t="s">
-        <v>473</v>
+      <c r="A78" s="1" t="s">
+        <v>504</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C78" s="10">
+      <c r="C78" s="8">
         <v>6</v>
       </c>
       <c r="D78" s="4" t="s">
@@ -6404,7 +6404,7 @@
       <c r="F78" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G78" s="8" t="s">
+      <c r="G78" s="6" t="s">
         <v>159</v>
       </c>
       <c r="H78" s="1" t="s">
@@ -6421,13 +6421,13 @@
       </c>
     </row>
     <row r="79" spans="1:12" ht="25.5">
-      <c r="A79" s="3" t="s">
-        <v>474</v>
+      <c r="A79" s="1" t="s">
+        <v>505</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C79" s="10">
+      <c r="C79" s="8">
         <v>7</v>
       </c>
       <c r="D79" s="4" t="s">
@@ -6439,7 +6439,7 @@
       <c r="F79" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G79" s="8" t="s">
+      <c r="G79" s="6" t="s">
         <v>161</v>
       </c>
       <c r="H79" s="1" t="s">
@@ -6456,13 +6456,13 @@
       </c>
     </row>
     <row r="80" spans="1:12" ht="25.5">
-      <c r="A80" s="3" t="s">
-        <v>475</v>
+      <c r="A80" s="1" t="s">
+        <v>506</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C80" s="10">
+      <c r="C80" s="8">
         <v>1</v>
       </c>
       <c r="D80" s="4" t="s">
@@ -6474,7 +6474,7 @@
       <c r="F80" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G80" s="8" t="s">
+      <c r="G80" s="6" t="s">
         <v>163</v>
       </c>
       <c r="H80" s="1" t="s">
@@ -6491,13 +6491,13 @@
       </c>
     </row>
     <row r="81" spans="1:12">
-      <c r="A81" s="3" t="s">
-        <v>476</v>
+      <c r="A81" s="1" t="s">
+        <v>507</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C81" s="10">
+      <c r="C81" s="8">
         <v>2</v>
       </c>
       <c r="D81" s="4" t="s">
@@ -6509,7 +6509,7 @@
       <c r="F81" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G81" s="8" t="s">
+      <c r="G81" s="6" t="s">
         <v>165</v>
       </c>
       <c r="H81" s="1" t="s">
@@ -6529,13 +6529,13 @@
       </c>
     </row>
     <row r="82" spans="1:12" ht="38.25">
-      <c r="A82" s="3" t="s">
-        <v>477</v>
+      <c r="A82" s="1" t="s">
+        <v>508</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C82" s="10">
+      <c r="C82" s="8">
         <v>3</v>
       </c>
       <c r="D82" s="4" t="s">
@@ -6547,7 +6547,7 @@
       <c r="F82" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G82" s="8" t="s">
+      <c r="G82" s="6" t="s">
         <v>167</v>
       </c>
       <c r="H82" s="1" t="s">
@@ -6567,13 +6567,13 @@
       </c>
     </row>
     <row r="83" spans="1:12">
-      <c r="A83" s="3" t="s">
-        <v>478</v>
+      <c r="A83" s="1" t="s">
+        <v>509</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C83" s="10">
+      <c r="C83" s="8">
         <v>4</v>
       </c>
       <c r="D83" s="4" t="s">
@@ -6585,7 +6585,7 @@
       <c r="F83" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G83" s="8" t="s">
+      <c r="G83" s="6" t="s">
         <v>23</v>
       </c>
       <c r="H83" s="1" t="s">
@@ -6602,13 +6602,13 @@
       </c>
     </row>
     <row r="84" spans="1:12">
-      <c r="A84" s="3" t="s">
-        <v>479</v>
+      <c r="A84" s="1" t="s">
+        <v>510</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C84" s="10">
+      <c r="C84" s="8">
         <v>5</v>
       </c>
       <c r="D84" s="4" t="s">
@@ -6620,7 +6620,7 @@
       <c r="F84" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G84" s="8" t="s">
+      <c r="G84" s="6" t="s">
         <v>25</v>
       </c>
       <c r="H84" s="1" t="s">
@@ -6637,13 +6637,13 @@
       </c>
     </row>
     <row r="85" spans="1:12">
-      <c r="A85" s="3" t="s">
-        <v>480</v>
+      <c r="A85" s="1" t="s">
+        <v>511</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C85" s="10">
+      <c r="C85" s="8">
         <v>6</v>
       </c>
       <c r="D85" s="4" t="s">
@@ -6655,7 +6655,7 @@
       <c r="F85" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G85" s="8" t="s">
+      <c r="G85" s="6" t="s">
         <v>168</v>
       </c>
       <c r="H85" s="1" t="s">
@@ -6672,13 +6672,13 @@
       </c>
     </row>
     <row r="86" spans="1:12" ht="25.5">
-      <c r="A86" s="3" t="s">
-        <v>481</v>
+      <c r="A86" s="1" t="s">
+        <v>512</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C86" s="10">
+      <c r="C86" s="8">
         <v>7</v>
       </c>
       <c r="D86" s="4" t="s">
@@ -6690,7 +6690,7 @@
       <c r="F86" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G86" s="8" t="s">
+      <c r="G86" s="6" t="s">
         <v>169</v>
       </c>
       <c r="H86" s="1" t="s">
@@ -6707,13 +6707,13 @@
       </c>
     </row>
     <row r="87" spans="1:12" ht="25.5">
-      <c r="A87" s="3" t="s">
-        <v>482</v>
+      <c r="A87" s="1" t="s">
+        <v>513</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C87" s="10">
+      <c r="C87" s="8">
         <v>8</v>
       </c>
       <c r="D87" s="4" t="s">
@@ -6725,7 +6725,7 @@
       <c r="F87" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G87" s="8" t="s">
+      <c r="G87" s="6" t="s">
         <v>170</v>
       </c>
       <c r="H87" s="1" t="s">
@@ -6742,13 +6742,13 @@
       </c>
     </row>
     <row r="88" spans="1:12">
-      <c r="A88" s="3" t="s">
-        <v>483</v>
+      <c r="A88" s="1" t="s">
+        <v>514</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C88" s="10">
+      <c r="C88" s="8">
         <v>9</v>
       </c>
       <c r="D88" s="4" t="s">
@@ -6760,7 +6760,7 @@
       <c r="F88" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G88" s="8" t="s">
+      <c r="G88" s="6" t="s">
         <v>113</v>
       </c>
       <c r="H88" s="1" t="s">
@@ -6777,13 +6777,13 @@
       </c>
     </row>
     <row r="89" spans="1:12">
-      <c r="A89" s="3" t="s">
-        <v>484</v>
+      <c r="A89" s="1" t="s">
+        <v>515</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C89" s="10">
+      <c r="C89" s="8">
         <v>10</v>
       </c>
       <c r="D89" s="4" t="s">
@@ -6795,7 +6795,7 @@
       <c r="F89" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G89" s="8" t="s">
+      <c r="G89" s="6" t="s">
         <v>172</v>
       </c>
       <c r="H89" s="1" t="s">
@@ -6812,13 +6812,13 @@
       </c>
     </row>
     <row r="90" spans="1:12">
-      <c r="A90" s="3" t="s">
-        <v>485</v>
+      <c r="A90" s="1" t="s">
+        <v>516</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C90" s="10">
+      <c r="C90" s="8">
         <v>11</v>
       </c>
       <c r="D90" s="4" t="s">
@@ -6830,7 +6830,7 @@
       <c r="F90" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G90" s="8" t="s">
+      <c r="G90" s="6" t="s">
         <v>174</v>
       </c>
       <c r="H90" s="1" t="s">
@@ -6850,13 +6850,13 @@
       </c>
     </row>
     <row r="91" spans="1:12">
-      <c r="A91" s="3" t="s">
-        <v>486</v>
+      <c r="A91" s="1" t="s">
+        <v>517</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C91" s="10">
+      <c r="C91" s="8">
         <v>12</v>
       </c>
       <c r="D91" s="4" t="s">
@@ -6868,7 +6868,7 @@
       <c r="F91" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G91" s="8" t="s">
+      <c r="G91" s="6" t="s">
         <v>176</v>
       </c>
       <c r="H91" s="1" t="s">
@@ -6888,13 +6888,13 @@
       </c>
     </row>
     <row r="92" spans="1:12">
-      <c r="A92" s="3" t="s">
-        <v>487</v>
+      <c r="A92" s="1" t="s">
+        <v>518</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C92" s="10">
+      <c r="C92" s="8">
         <v>13</v>
       </c>
       <c r="D92" s="4" t="s">
@@ -6906,7 +6906,7 @@
       <c r="F92" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G92" s="8" t="s">
+      <c r="G92" s="6" t="s">
         <v>178</v>
       </c>
       <c r="H92" s="1" t="s">
@@ -6923,13 +6923,13 @@
       </c>
     </row>
     <row r="93" spans="1:12" ht="25.5">
-      <c r="A93" s="3" t="s">
-        <v>488</v>
+      <c r="A93" s="1" t="s">
+        <v>519</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C93" s="10">
+      <c r="C93" s="8">
         <v>14</v>
       </c>
       <c r="D93" s="4" t="s">
@@ -6941,7 +6941,7 @@
       <c r="F93" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G93" s="8" t="s">
+      <c r="G93" s="6" t="s">
         <v>180</v>
       </c>
       <c r="H93" s="1" t="s">
@@ -6958,13 +6958,13 @@
       </c>
     </row>
     <row r="94" spans="1:12">
-      <c r="A94" s="3" t="s">
-        <v>489</v>
+      <c r="A94" s="1" t="s">
+        <v>520</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C94" s="10">
+      <c r="C94" s="8">
         <v>15</v>
       </c>
       <c r="D94" s="4" t="s">
@@ -6976,7 +6976,7 @@
       <c r="F94" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G94" s="8" t="s">
+      <c r="G94" s="6" t="s">
         <v>182</v>
       </c>
       <c r="H94" s="1" t="s">
@@ -6996,13 +6996,13 @@
       </c>
     </row>
     <row r="95" spans="1:12">
-      <c r="A95" s="3" t="s">
-        <v>490</v>
+      <c r="A95" s="1" t="s">
+        <v>521</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C95" s="10">
+      <c r="C95" s="8">
         <v>16</v>
       </c>
       <c r="D95" s="4" t="s">
@@ -7014,7 +7014,7 @@
       <c r="F95" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G95" s="8" t="s">
+      <c r="G95" s="6" t="s">
         <v>184</v>
       </c>
       <c r="H95" s="1" t="s">
@@ -7034,13 +7034,13 @@
       </c>
     </row>
     <row r="96" spans="1:12" ht="25.5">
-      <c r="A96" s="3" t="s">
-        <v>491</v>
+      <c r="A96" s="1" t="s">
+        <v>522</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C96" s="10">
+      <c r="C96" s="8">
         <v>17</v>
       </c>
       <c r="D96" s="4" t="s">
@@ -7052,7 +7052,7 @@
       <c r="F96" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G96" s="8" t="s">
+      <c r="G96" s="6" t="s">
         <v>186</v>
       </c>
       <c r="H96" s="1" t="s">
@@ -7072,13 +7072,13 @@
       </c>
     </row>
     <row r="97" spans="1:12" ht="25.5">
-      <c r="A97" s="3" t="s">
-        <v>492</v>
+      <c r="A97" s="1" t="s">
+        <v>523</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C97" s="10">
+      <c r="C97" s="8">
         <v>18</v>
       </c>
       <c r="D97" s="4" t="s">
@@ -7090,7 +7090,7 @@
       <c r="F97" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G97" s="8" t="s">
+      <c r="G97" s="6" t="s">
         <v>188</v>
       </c>
       <c r="H97" s="1" t="s">
@@ -7107,13 +7107,13 @@
       </c>
     </row>
     <row r="98" spans="1:12" ht="25.5">
-      <c r="A98" s="3" t="s">
-        <v>493</v>
+      <c r="A98" s="1" t="s">
+        <v>524</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C98" s="10">
+      <c r="C98" s="8">
         <v>19</v>
       </c>
       <c r="D98" s="4" t="s">
@@ -7125,7 +7125,7 @@
       <c r="F98" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G98" s="8" t="s">
+      <c r="G98" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H98" s="1" t="s">
@@ -7145,13 +7145,13 @@
       </c>
     </row>
     <row r="99" spans="1:12">
-      <c r="A99" s="3" t="s">
-        <v>494</v>
+      <c r="A99" s="1" t="s">
+        <v>525</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C99" s="10">
+      <c r="C99" s="8">
         <v>20</v>
       </c>
       <c r="D99" s="4" t="s">
@@ -7163,7 +7163,7 @@
       <c r="F99" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G99" s="8" t="s">
+      <c r="G99" s="6" t="s">
         <v>192</v>
       </c>
       <c r="H99" s="1" t="s">
@@ -7183,13 +7183,13 @@
       </c>
     </row>
     <row r="100" spans="1:12">
-      <c r="A100" s="3" t="s">
-        <v>495</v>
+      <c r="A100" s="1" t="s">
+        <v>526</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C100" s="10">
+      <c r="C100" s="8">
         <v>21</v>
       </c>
       <c r="D100" s="4" t="s">
@@ -7201,7 +7201,7 @@
       <c r="F100" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G100" s="8" t="s">
+      <c r="G100" s="6" t="s">
         <v>194</v>
       </c>
       <c r="H100" s="1" t="s">
@@ -7218,13 +7218,13 @@
       </c>
     </row>
     <row r="101" spans="1:12" ht="25.5">
-      <c r="A101" s="3" t="s">
-        <v>496</v>
+      <c r="A101" s="1" t="s">
+        <v>527</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C101" s="10">
+      <c r="C101" s="8">
         <v>22</v>
       </c>
       <c r="D101" s="4" t="s">
@@ -7236,7 +7236,7 @@
       <c r="F101" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G101" s="8" t="s">
+      <c r="G101" s="6" t="s">
         <v>196</v>
       </c>
       <c r="H101" s="1" t="s">
@@ -7253,13 +7253,13 @@
       </c>
     </row>
     <row r="102" spans="1:12" ht="25.5">
-      <c r="A102" s="3" t="s">
-        <v>497</v>
+      <c r="A102" s="1" t="s">
+        <v>528</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C102" s="10">
+      <c r="C102" s="8">
         <v>23</v>
       </c>
       <c r="D102" s="4" t="s">
@@ -7271,7 +7271,7 @@
       <c r="F102" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G102" s="8" t="s">
+      <c r="G102" s="6" t="s">
         <v>198</v>
       </c>
       <c r="H102" s="1" t="s">
@@ -7288,13 +7288,13 @@
       </c>
     </row>
     <row r="103" spans="1:12">
-      <c r="A103" s="3" t="s">
-        <v>498</v>
+      <c r="A103" s="1" t="s">
+        <v>529</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C103" s="10">
+      <c r="C103" s="8">
         <v>24</v>
       </c>
       <c r="D103" s="4" t="s">
@@ -7306,7 +7306,7 @@
       <c r="F103" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G103" s="8" t="s">
+      <c r="G103" s="6" t="s">
         <v>200</v>
       </c>
       <c r="H103" s="1" t="s">
@@ -7323,13 +7323,13 @@
       </c>
     </row>
     <row r="104" spans="1:12">
-      <c r="A104" s="3" t="s">
-        <v>499</v>
+      <c r="A104" s="1" t="s">
+        <v>530</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C104" s="10">
+      <c r="C104" s="8">
         <v>25</v>
       </c>
       <c r="D104" s="4" t="s">
@@ -7341,7 +7341,7 @@
       <c r="F104" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G104" s="8" t="s">
+      <c r="G104" s="6" t="s">
         <v>202</v>
       </c>
       <c r="H104" s="1" t="s">
@@ -7361,13 +7361,13 @@
       </c>
     </row>
     <row r="105" spans="1:12" ht="25.5">
-      <c r="A105" s="3" t="s">
-        <v>500</v>
+      <c r="A105" s="1" t="s">
+        <v>531</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C105" s="10">
+      <c r="C105" s="8">
         <v>26</v>
       </c>
       <c r="D105" s="4" t="s">
@@ -7379,7 +7379,7 @@
       <c r="F105" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G105" s="8" t="s">
+      <c r="G105" s="6" t="s">
         <v>204</v>
       </c>
       <c r="H105" s="1" t="s">
@@ -7396,13 +7396,13 @@
       </c>
     </row>
     <row r="106" spans="1:12">
-      <c r="A106" s="3" t="s">
-        <v>501</v>
+      <c r="A106" s="1" t="s">
+        <v>532</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C106" s="10">
+      <c r="C106" s="8">
         <v>1</v>
       </c>
       <c r="D106" s="3" t="s">
@@ -7414,7 +7414,7 @@
       <c r="F106" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G106" s="8" t="s">
+      <c r="G106" s="6" t="s">
         <v>207</v>
       </c>
       <c r="H106" s="1" t="s">
@@ -7431,13 +7431,13 @@
       </c>
     </row>
     <row r="107" spans="1:12">
-      <c r="A107" s="3" t="s">
-        <v>502</v>
+      <c r="A107" s="1" t="s">
+        <v>533</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C107" s="10">
+      <c r="C107" s="8">
         <v>2</v>
       </c>
       <c r="D107" s="3" t="s">
@@ -7449,7 +7449,7 @@
       <c r="F107" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G107" s="8" t="s">
+      <c r="G107" s="6" t="s">
         <v>210</v>
       </c>
       <c r="H107" s="1" t="s">
@@ -7466,13 +7466,13 @@
       </c>
     </row>
     <row r="108" spans="1:12">
-      <c r="A108" s="3" t="s">
-        <v>503</v>
+      <c r="A108" s="1" t="s">
+        <v>534</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C108" s="10">
+      <c r="C108" s="8">
         <v>3</v>
       </c>
       <c r="D108" s="3" t="s">
@@ -7484,7 +7484,7 @@
       <c r="F108" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="G108" s="8" t="s">
+      <c r="G108" s="6" t="s">
         <v>214</v>
       </c>
       <c r="H108" s="1" t="s">
@@ -7501,13 +7501,13 @@
       </c>
     </row>
     <row r="109" spans="1:12">
-      <c r="A109" s="3" t="s">
-        <v>504</v>
+      <c r="A109" s="1" t="s">
+        <v>535</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C109" s="10">
+      <c r="C109" s="8">
         <v>4</v>
       </c>
       <c r="D109" s="3" t="s">
@@ -7519,7 +7519,7 @@
       <c r="F109" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G109" s="8" t="s">
+      <c r="G109" s="6" t="s">
         <v>217</v>
       </c>
       <c r="H109" s="1" t="s">
@@ -7536,13 +7536,13 @@
       </c>
     </row>
     <row r="110" spans="1:12" ht="25.5">
-      <c r="A110" s="3" t="s">
-        <v>505</v>
+      <c r="A110" s="1" t="s">
+        <v>536</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C110" s="10">
+      <c r="C110" s="8">
         <v>5</v>
       </c>
       <c r="D110" s="3" t="s">
@@ -7554,7 +7554,7 @@
       <c r="F110" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G110" s="8" t="s">
+      <c r="G110" s="6" t="s">
         <v>220</v>
       </c>
       <c r="H110" s="1" t="s">
@@ -7571,13 +7571,13 @@
       </c>
     </row>
     <row r="111" spans="1:12">
-      <c r="A111" s="3" t="s">
-        <v>506</v>
+      <c r="A111" s="1" t="s">
+        <v>537</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C111" s="10">
+      <c r="C111" s="8">
         <v>6</v>
       </c>
       <c r="D111" s="4" t="s">
@@ -7589,7 +7589,7 @@
       <c r="F111" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="G111" s="8" t="s">
+      <c r="G111" s="6" t="s">
         <v>223</v>
       </c>
       <c r="H111" s="1" t="s">
@@ -7606,13 +7606,13 @@
       </c>
     </row>
     <row r="112" spans="1:12">
-      <c r="A112" s="3" t="s">
-        <v>507</v>
+      <c r="A112" s="1" t="s">
+        <v>538</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C112" s="10">
+      <c r="C112" s="8">
         <v>7</v>
       </c>
       <c r="D112" s="4" t="s">
@@ -7624,7 +7624,7 @@
       <c r="F112" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="G112" s="8" t="s">
+      <c r="G112" s="6" t="s">
         <v>225</v>
       </c>
       <c r="H112" s="1" t="s">
@@ -7641,13 +7641,13 @@
       </c>
     </row>
     <row r="113" spans="1:12">
-      <c r="A113" s="3" t="s">
-        <v>508</v>
+      <c r="A113" s="1" t="s">
+        <v>539</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C113" s="10">
+      <c r="C113" s="8">
         <v>8</v>
       </c>
       <c r="D113" s="4" t="s">
@@ -7659,7 +7659,7 @@
       <c r="F113" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="G113" s="8" t="s">
+      <c r="G113" s="6" t="s">
         <v>227</v>
       </c>
       <c r="H113" s="1" t="s">
@@ -7676,13 +7676,13 @@
       </c>
     </row>
     <row r="114" spans="1:12" ht="25.5">
-      <c r="A114" s="3" t="s">
-        <v>509</v>
+      <c r="A114" s="1" t="s">
+        <v>540</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C114" s="10">
+      <c r="C114" s="8">
         <v>9</v>
       </c>
       <c r="D114" s="4" t="s">
@@ -7694,7 +7694,7 @@
       <c r="F114" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="G114" s="8" t="s">
+      <c r="G114" s="6" t="s">
         <v>229</v>
       </c>
       <c r="H114" s="1" t="s">
@@ -7711,13 +7711,13 @@
       </c>
     </row>
     <row r="115" spans="1:12" ht="25.5">
-      <c r="A115" s="3" t="s">
-        <v>510</v>
+      <c r="A115" s="1" t="s">
+        <v>541</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C115" s="10">
+      <c r="C115" s="8">
         <v>10</v>
       </c>
       <c r="D115" s="4" t="s">
@@ -7729,7 +7729,7 @@
       <c r="F115" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="G115" s="8" t="s">
+      <c r="G115" s="6" t="s">
         <v>231</v>
       </c>
       <c r="H115" s="1" t="s">
@@ -7746,13 +7746,13 @@
       </c>
     </row>
     <row r="116" spans="1:12" ht="25.5">
-      <c r="A116" s="3" t="s">
-        <v>511</v>
+      <c r="A116" s="1" t="s">
+        <v>542</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C116" s="10">
+      <c r="C116" s="8">
         <v>11</v>
       </c>
       <c r="D116" s="4" t="s">
@@ -7764,7 +7764,7 @@
       <c r="F116" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="G116" s="8" t="s">
+      <c r="G116" s="6" t="s">
         <v>233</v>
       </c>
       <c r="H116" s="1" t="s">
@@ -7781,13 +7781,13 @@
       </c>
     </row>
     <row r="117" spans="1:12" ht="25.5">
-      <c r="A117" s="3" t="s">
-        <v>512</v>
+      <c r="A117" s="1" t="s">
+        <v>543</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C117" s="10">
+      <c r="C117" s="8">
         <v>12</v>
       </c>
       <c r="D117" s="4" t="s">
@@ -7799,7 +7799,7 @@
       <c r="F117" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="G117" s="8" t="s">
+      <c r="G117" s="6" t="s">
         <v>236</v>
       </c>
       <c r="H117" s="1" t="s">
@@ -7816,13 +7816,13 @@
       </c>
     </row>
     <row r="118" spans="1:12" ht="38.25">
-      <c r="A118" s="3" t="s">
-        <v>513</v>
+      <c r="A118" s="1" t="s">
+        <v>544</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C118" s="10">
+      <c r="C118" s="8">
         <v>13</v>
       </c>
       <c r="D118" s="4" t="s">
@@ -7834,7 +7834,7 @@
       <c r="F118" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G118" s="8" t="s">
+      <c r="G118" s="6" t="s">
         <v>238</v>
       </c>
       <c r="H118" s="1" t="s">
@@ -7851,13 +7851,13 @@
       </c>
     </row>
     <row r="119" spans="1:12">
-      <c r="A119" s="3" t="s">
-        <v>514</v>
+      <c r="A119" s="1" t="s">
+        <v>545</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C119" s="10">
+      <c r="C119" s="8">
         <v>14</v>
       </c>
       <c r="D119" s="4" t="s">
@@ -7869,7 +7869,7 @@
       <c r="F119" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G119" s="8" t="s">
+      <c r="G119" s="6" t="s">
         <v>240</v>
       </c>
       <c r="H119" s="1" t="s">
@@ -7886,13 +7886,13 @@
       </c>
     </row>
     <row r="120" spans="1:12" ht="51">
-      <c r="A120" s="3" t="s">
-        <v>515</v>
+      <c r="A120" s="1" t="s">
+        <v>546</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C120" s="10">
+      <c r="C120" s="8">
         <v>15</v>
       </c>
       <c r="D120" s="4" t="s">
@@ -7904,7 +7904,7 @@
       <c r="F120" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="G120" s="8" t="s">
+      <c r="G120" s="6" t="s">
         <v>242</v>
       </c>
       <c r="H120" s="1" t="s">
@@ -7921,13 +7921,13 @@
       </c>
     </row>
     <row r="121" spans="1:12" ht="25.5">
-      <c r="A121" s="3" t="s">
-        <v>516</v>
+      <c r="A121" s="1" t="s">
+        <v>547</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C121" s="10">
+      <c r="C121" s="8">
         <v>16</v>
       </c>
       <c r="D121" s="4" t="s">
@@ -7939,7 +7939,7 @@
       <c r="F121" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G121" s="8" t="s">
+      <c r="G121" s="6" t="s">
         <v>244</v>
       </c>
       <c r="H121" s="1" t="s">
@@ -7956,13 +7956,13 @@
       </c>
     </row>
     <row r="122" spans="1:12">
-      <c r="A122" s="3" t="s">
-        <v>517</v>
+      <c r="A122" s="1" t="s">
+        <v>548</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C122" s="10">
+      <c r="C122" s="8">
         <v>17</v>
       </c>
       <c r="D122" s="4" t="s">
@@ -7974,7 +7974,7 @@
       <c r="F122" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="G122" s="8" t="s">
+      <c r="G122" s="6" t="s">
         <v>246</v>
       </c>
       <c r="H122" s="1" t="s">
@@ -7991,13 +7991,13 @@
       </c>
     </row>
     <row r="123" spans="1:12" ht="51">
-      <c r="A123" s="3" t="s">
-        <v>518</v>
+      <c r="A123" s="1" t="s">
+        <v>549</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C123" s="10">
+      <c r="C123" s="8">
         <v>18</v>
       </c>
       <c r="D123" s="4" t="s">
@@ -8009,7 +8009,7 @@
       <c r="F123" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G123" s="8" t="s">
+      <c r="G123" s="6" t="s">
         <v>248</v>
       </c>
       <c r="H123" s="1" t="s">
@@ -8026,13 +8026,13 @@
       </c>
     </row>
     <row r="124" spans="1:12" ht="51">
-      <c r="A124" s="3" t="s">
-        <v>519</v>
+      <c r="A124" s="1" t="s">
+        <v>550</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C124" s="10">
+      <c r="C124" s="8">
         <v>19</v>
       </c>
       <c r="D124" s="4" t="s">
@@ -8044,7 +8044,7 @@
       <c r="F124" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G124" s="8" t="s">
+      <c r="G124" s="6" t="s">
         <v>250</v>
       </c>
       <c r="H124" s="1" t="s">
@@ -8061,13 +8061,13 @@
       </c>
     </row>
     <row r="125" spans="1:12" ht="38.25">
-      <c r="A125" s="3" t="s">
-        <v>520</v>
+      <c r="A125" s="1" t="s">
+        <v>551</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C125" s="10">
+      <c r="C125" s="8">
         <v>20</v>
       </c>
       <c r="D125" s="4" t="s">
@@ -8079,7 +8079,7 @@
       <c r="F125" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="G125" s="8" t="s">
+      <c r="G125" s="6" t="s">
         <v>252</v>
       </c>
       <c r="H125" s="1" t="s">
@@ -8096,13 +8096,13 @@
       </c>
     </row>
     <row r="126" spans="1:12" ht="25.5">
-      <c r="A126" s="3" t="s">
-        <v>521</v>
+      <c r="A126" s="1" t="s">
+        <v>552</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C126" s="10">
+      <c r="C126" s="8">
         <v>21</v>
       </c>
       <c r="D126" s="4" t="s">
@@ -8114,7 +8114,7 @@
       <c r="F126" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G126" s="8" t="s">
+      <c r="G126" s="6" t="s">
         <v>254</v>
       </c>
       <c r="H126" s="1" t="s">
@@ -8131,13 +8131,13 @@
       </c>
     </row>
     <row r="127" spans="1:12" ht="25.5">
-      <c r="A127" s="3" t="s">
-        <v>522</v>
+      <c r="A127" s="1" t="s">
+        <v>553</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C127" s="10">
+      <c r="C127" s="8">
         <v>22</v>
       </c>
       <c r="D127" s="4" t="s">
@@ -8149,7 +8149,7 @@
       <c r="F127" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G127" s="8" t="s">
+      <c r="G127" s="6" t="s">
         <v>256</v>
       </c>
       <c r="H127" s="1" t="s">
@@ -8166,13 +8166,13 @@
       </c>
     </row>
     <row r="128" spans="1:12" ht="25.5">
-      <c r="A128" s="3" t="s">
-        <v>523</v>
+      <c r="A128" s="1" t="s">
+        <v>554</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C128" s="10">
+      <c r="C128" s="8">
         <v>23</v>
       </c>
       <c r="D128" s="4" t="s">
@@ -8184,7 +8184,7 @@
       <c r="F128" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G128" s="8" t="s">
+      <c r="G128" s="6" t="s">
         <v>258</v>
       </c>
       <c r="H128" s="1" t="s">
@@ -8201,13 +8201,13 @@
       </c>
     </row>
     <row r="129" spans="1:12" ht="25.5">
-      <c r="A129" s="3" t="s">
-        <v>524</v>
+      <c r="A129" s="1" t="s">
+        <v>555</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C129" s="10">
+      <c r="C129" s="8">
         <v>24</v>
       </c>
       <c r="D129" s="4" t="s">
@@ -8219,7 +8219,7 @@
       <c r="F129" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G129" s="8" t="s">
+      <c r="G129" s="6" t="s">
         <v>260</v>
       </c>
       <c r="H129" s="1" t="s">
@@ -8237,7 +8237,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>